<commit_message>
Updated arguments document, exploratory analysis, and problem model
</commit_message>
<xml_diff>
--- a/docs/2-Problem Model.xlsx
+++ b/docs/2-Problem Model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calvindelima/ds/bank-term-loan-prediction/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calvindelima/ds/bank-term-loan-prediction-github/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB80B03B-68A7-BA4A-9E07-AECA298593DC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0AD787-F85D-814D-B1F8-0C7EB9CE64AE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8540" yWindow="5440" windowWidth="28040" windowHeight="17040" xr2:uid="{054F7AF6-F6F7-CA43-8419-9B526FF8FE98}"/>
+    <workbookView xWindow="280" yWindow="680" windowWidth="28040" windowHeight="17040" xr2:uid="{054F7AF6-F6F7-CA43-8419-9B526FF8FE98}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamics" sheetId="4" r:id="rId1"/>
@@ -43,6 +43,8 @@
     <definedName name="MinCallDuraiton">Costs!$B$4</definedName>
     <definedName name="MinCallDuration">Costs!$B$4</definedName>
     <definedName name="NetBankInterest">Benefits!$B$10</definedName>
+    <definedName name="Population_Size">#REF!</definedName>
+    <definedName name="PopulationSize">#REF!</definedName>
     <definedName name="Revenue_Avg">Benefits!$B$16</definedName>
     <definedName name="Revenue_High">Benefits!$B$14</definedName>
     <definedName name="Revenue_Low">Benefits!$B$12</definedName>
@@ -733,7 +735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B15A00-FC3C-7045-A9E6-1266591F3F56}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1074,7 +1076,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1092,7 +1094,7 @@
         <v>35</v>
       </c>
       <c r="B1" s="35">
-        <v>1.2</v>
+        <v>2.1800000000000002</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1101,7 +1103,7 @@
       </c>
       <c r="B2" s="36">
         <f>Lift*ConversionRate</f>
-        <v>0.13200000000000001</v>
+        <v>0.23980000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1110,7 +1112,7 @@
       </c>
       <c r="B3" s="36">
         <f>B2-ConversionRate</f>
-        <v>2.2000000000000006E-2</v>
+        <v>0.12980000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -1154,15 +1156,15 @@
       </c>
       <c r="E6" s="29">
         <f>Lift*C6</f>
-        <v>187540.98360655736</v>
+        <v>340699.45355191256</v>
       </c>
       <c r="F6" s="25">
         <f>E6-A6</f>
-        <v>177540.98360655736</v>
+        <v>330699.45355191256</v>
       </c>
       <c r="G6" s="28">
         <f>F6-D6</f>
-        <v>31256.830601092894</v>
+        <v>184415.3005464481</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1176,23 +1178,23 @@
       </c>
       <c r="C7" s="26">
         <f t="shared" ref="C7:C15" si="1">B7*Lift*ConversionRate*Revenue_Avg</f>
-        <v>375081.96721311472</v>
+        <v>681398.90710382513</v>
       </c>
       <c r="D7" s="25">
         <f t="shared" ref="D7:D15" si="2">C7-A7</f>
-        <v>355081.96721311472</v>
+        <v>661398.90710382513</v>
       </c>
       <c r="E7" s="25">
         <f t="shared" ref="E7:E15" si="3">Lift*C7</f>
-        <v>450098.36065573763</v>
+        <v>1485449.6174863388</v>
       </c>
       <c r="F7" s="25">
         <f t="shared" ref="F7:F15" si="4">E7-A7</f>
-        <v>430098.36065573763</v>
+        <v>1465449.6174863388</v>
       </c>
       <c r="G7" s="28">
         <f t="shared" ref="G7:G15" si="5">F7-D7</f>
-        <v>75016.39344262291</v>
+        <v>804050.7103825137</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1206,23 +1208,23 @@
       </c>
       <c r="C8" s="26">
         <f t="shared" si="1"/>
-        <v>562622.95081967209</v>
+        <v>1022098.3606557377</v>
       </c>
       <c r="D8" s="25">
         <f t="shared" si="2"/>
-        <v>532622.95081967209</v>
+        <v>992098.36065573769</v>
       </c>
       <c r="E8" s="25">
         <f t="shared" si="3"/>
-        <v>675147.54098360648</v>
+        <v>2228174.4262295081</v>
       </c>
       <c r="F8" s="25">
         <f t="shared" si="4"/>
-        <v>645147.54098360648</v>
+        <v>2198174.4262295081</v>
       </c>
       <c r="G8" s="28">
         <f t="shared" si="5"/>
-        <v>112524.59016393439</v>
+        <v>1206076.0655737706</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1236,23 +1238,23 @@
       </c>
       <c r="C9" s="26">
         <f t="shared" si="1"/>
-        <v>750163.93442622945</v>
+        <v>1362797.8142076503</v>
       </c>
       <c r="D9" s="25">
         <f t="shared" si="2"/>
-        <v>710163.93442622945</v>
+        <v>1322797.8142076503</v>
       </c>
       <c r="E9" s="25">
         <f t="shared" si="3"/>
-        <v>900196.72131147527</v>
+        <v>2970899.2349726777</v>
       </c>
       <c r="F9" s="25">
         <f t="shared" si="4"/>
-        <v>860196.72131147527</v>
+        <v>2930899.2349726777</v>
       </c>
       <c r="G9" s="28">
         <f t="shared" si="5"/>
-        <v>150032.78688524582</v>
+        <v>1608101.4207650274</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.2">
@@ -1266,23 +1268,23 @@
       </c>
       <c r="C10" s="32">
         <f t="shared" si="1"/>
-        <v>937704.91803278681</v>
+        <v>1703497.2677595629</v>
       </c>
       <c r="D10" s="30">
         <f t="shared" si="2"/>
-        <v>887704.91803278681</v>
+        <v>1653497.2677595629</v>
       </c>
       <c r="E10" s="30">
         <f t="shared" si="3"/>
-        <v>1125245.9016393442</v>
+        <v>3713624.0437158477</v>
       </c>
       <c r="F10" s="30">
         <f t="shared" si="4"/>
-        <v>1075245.9016393442</v>
+        <v>3663624.0437158477</v>
       </c>
       <c r="G10" s="33">
         <f t="shared" si="5"/>
-        <v>187540.98360655736</v>
+        <v>2010126.7759562847</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1296,23 +1298,23 @@
       </c>
       <c r="C11" s="26">
         <f t="shared" si="1"/>
-        <v>1125245.9016393442</v>
+        <v>2044196.7213114754</v>
       </c>
       <c r="D11" s="25">
         <f t="shared" si="2"/>
-        <v>1065245.9016393442</v>
+        <v>1984196.7213114754</v>
       </c>
       <c r="E11" s="25">
         <f t="shared" si="3"/>
-        <v>1350295.081967213</v>
+        <v>4456348.8524590163</v>
       </c>
       <c r="F11" s="25">
         <f t="shared" si="4"/>
-        <v>1290295.081967213</v>
+        <v>4396348.8524590163</v>
       </c>
       <c r="G11" s="28">
         <f t="shared" si="5"/>
-        <v>225049.18032786879</v>
+        <v>2412152.1311475411</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1326,23 +1328,23 @@
       </c>
       <c r="C12" s="26">
         <f t="shared" si="1"/>
-        <v>1312786.8852459013</v>
+        <v>2384896.1748633878</v>
       </c>
       <c r="D12" s="25">
         <f t="shared" si="2"/>
-        <v>1242786.8852459013</v>
+        <v>2314896.1748633878</v>
       </c>
       <c r="E12" s="25">
         <f t="shared" si="3"/>
-        <v>1575344.2622950815</v>
+        <v>5199073.6612021858</v>
       </c>
       <c r="F12" s="25">
         <f t="shared" si="4"/>
-        <v>1505344.2622950815</v>
+        <v>5129073.6612021858</v>
       </c>
       <c r="G12" s="28">
         <f t="shared" si="5"/>
-        <v>262557.37704918021</v>
+        <v>2814177.486338798</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1356,23 +1358,23 @@
       </c>
       <c r="C13" s="26">
         <f t="shared" si="1"/>
-        <v>1500327.8688524589</v>
+        <v>2725595.6284153005</v>
       </c>
       <c r="D13" s="25">
         <f t="shared" si="2"/>
-        <v>1420327.8688524589</v>
+        <v>2645595.6284153005</v>
       </c>
       <c r="E13" s="25">
         <f t="shared" si="3"/>
-        <v>1800393.4426229505</v>
+        <v>5941798.4699453553</v>
       </c>
       <c r="F13" s="25">
         <f t="shared" si="4"/>
-        <v>1720393.4426229505</v>
+        <v>5861798.4699453553</v>
       </c>
       <c r="G13" s="28">
         <f t="shared" si="5"/>
-        <v>300065.57377049164</v>
+        <v>3216202.8415300548</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1386,23 +1388,23 @@
       </c>
       <c r="C14" s="26">
         <f t="shared" si="1"/>
-        <v>1687868.852459016</v>
+        <v>3066295.0819672127</v>
       </c>
       <c r="D14" s="25">
         <f t="shared" si="2"/>
-        <v>1597868.852459016</v>
+        <v>2976295.0819672127</v>
       </c>
       <c r="E14" s="25">
         <f t="shared" si="3"/>
-        <v>2025442.6229508191</v>
+        <v>6684523.2786885239</v>
       </c>
       <c r="F14" s="25">
         <f t="shared" si="4"/>
-        <v>1935442.6229508191</v>
+        <v>6594523.2786885239</v>
       </c>
       <c r="G14" s="28">
         <f t="shared" si="5"/>
-        <v>337573.77049180306</v>
+        <v>3618228.1967213112</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1416,23 +1418,23 @@
       </c>
       <c r="C15" s="26">
         <f t="shared" si="1"/>
-        <v>1875409.8360655736</v>
+        <v>3406994.5355191259</v>
       </c>
       <c r="D15" s="25">
         <f t="shared" si="2"/>
-        <v>1775409.8360655736</v>
+        <v>3306994.5355191259</v>
       </c>
       <c r="E15" s="25">
         <f t="shared" si="3"/>
-        <v>2250491.8032786883</v>
+        <v>7427248.0874316953</v>
       </c>
       <c r="F15" s="25">
         <f t="shared" si="4"/>
-        <v>2150491.8032786883</v>
+        <v>7327248.0874316953</v>
       </c>
       <c r="G15" s="28">
         <f t="shared" si="5"/>
-        <v>375081.96721311472</v>
+        <v>4020253.5519125694</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>